<commit_message>
Get reports for all ticket types
</commit_message>
<xml_diff>
--- a/Reports/eh_and_s_environmental_health_and_safety.xlsx
+++ b/Reports/eh_and_s_environmental_health_and_safety.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>TicketID</t>
   </si>
@@ -49,31 +49,43 @@
     <t>This could be a safety risk</t>
   </si>
   <si>
+    <t>241</t>
+  </si>
+  <si>
+    <t>EH &amp; S - Environmental Health &amp; Safety</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>2017-08-15T09:16:49.403000</t>
+  </si>
+  <si>
+    <t>Vincent Chov</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>2017-08-15T09:17:13.210000</t>
+  </si>
+  <si>
+    <t>CT - PSI Hartford Office</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>238</t>
   </si>
   <si>
-    <t>EH &amp; S - Environmental Health &amp; Safety</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>2017-08-14T16:27:27.013000</t>
   </si>
   <si>
-    <t>Vincent Chov</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>2017-08-14T16:27:27.163000</t>
-  </si>
-  <si>
-    <t>CT - PSI Hartford Office</t>
+    <t>2017-08-14T16:27:57.897000</t>
   </si>
   <si>
     <t>No</t>
@@ -416,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -495,6 +507,41 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>